<commit_message>
Latest Opp and Eng Changes
</commit_message>
<xml_diff>
--- a/TestData/T1232_NBCFormSubmitforReview.xlsx
+++ b/TestData/T1232_NBCFormSubmitforReview.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgoyal0427\source\repos\SalesForce_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CB95B0-FC63-4704-AEAF-8CC3FCE437FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="8565" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -23,20 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="177">
   <si>
     <t>Client</t>
   </si>
@@ -317,9 +310,6 @@
     <t>HL Capital, Inc.</t>
   </si>
   <si>
-    <t>Emre Abale</t>
-  </si>
-  <si>
     <t>Techno Coatings, Inc.</t>
   </si>
   <si>
@@ -347,9 +337,6 @@
     <t>Abale</t>
   </si>
   <si>
-    <t>Opportunity Overview: Please answer the Public M&amp;A question., Opportunity Overview: Please confirm that a group head has approved prior to submitting to the committee., Overview and Financials: Transaction Overview, Overview and Financials: Current Status, Overview and Financials: Company Description, Overview and Financials: Cross-border Angle, Overview and Financials: Asia Angle, Overview and Financials: Real Estate Angle, Overview and Financials: Ownership Structure &amp; Capital Structure, Overview and Financials: Total Debt(MM), Overview and Financials: Have the financials been subject to an audit?, Overview and Financials: Estimated Valuation (MM), Overview and Financials: Valuation Expectations, Overview and Financials: Risk Factors, Fees: Estimated Fee (MM), Fees: Fee Structure, Fees: Lockups on Future M&amp;A or Financing Work, Fees: Referral Fee Owed, Pre-Pitch: Will there be a pitch?, Pre-Pitch: Existing or Repeat Client?, Pre-Pitch: Please identify Houlihan Lokey's competition., Pre-Pitch: Have you checked Salesforce for existing relationships?, Pre-Pitch: Would the Opportunity benefit from TAS Assistance?, Pre-Pitch: If known, identify the name(s) of the client’s outside counsel and/or other advisors (If any), Financing Checklist: Has the Capital Markets Group been consulted regarding financing or capital structure?, Financing Checklist: Please summarize the existing financial arrangements., Fairness Checklist: Is there a potential Fairness Opinion component to this assignment?, Administrative: Restricted List?, Administrative: Conflicts Check not requested yet - Please return to the Opportunity and request a Conflicts Check., Administrative: Please answer all Conflicts Check Information questions.</t>
-  </si>
-  <si>
     <t>caoUser</t>
   </si>
   <si>
@@ -357,12 +344,228 @@
   </si>
   <si>
     <t>Alexander Odysseos</t>
+  </si>
+  <si>
+    <t>Mark Fisher</t>
+  </si>
+  <si>
+    <t>ValTotalDebt</t>
+  </si>
+  <si>
+    <t>ValEstValuation</t>
+  </si>
+  <si>
+    <t>ValCurrentStatus</t>
+  </si>
+  <si>
+    <t>ValValuationExp</t>
+  </si>
+  <si>
+    <t>ValCompDesc</t>
+  </si>
+  <si>
+    <t>ValRealEstate</t>
+  </si>
+  <si>
+    <t>ValOwnership</t>
+  </si>
+  <si>
+    <t>ValAsiaAngle</t>
+  </si>
+  <si>
+    <t>ValInternational</t>
+  </si>
+  <si>
+    <t>ValRiskFact</t>
+  </si>
+  <si>
+    <t>ValCapMkt</t>
+  </si>
+  <si>
+    <t>ValExistingFin</t>
+  </si>
+  <si>
+    <t>Financing Checklist: Please summarize the existing financial arrangements.</t>
+  </si>
+  <si>
+    <t>Financing Checklist: Has the Capital Markets Group been consulted regarding financing or capital structure?</t>
+  </si>
+  <si>
+    <t>ValFinSub</t>
+  </si>
+  <si>
+    <t>Financials: Add min 2 Historical or current and future Financial records when submitting the NBC form</t>
+  </si>
+  <si>
+    <t>ValNoFin</t>
+  </si>
+  <si>
+    <t>ValRetainer</t>
+  </si>
+  <si>
+    <t>ValRetainerFee</t>
+  </si>
+  <si>
+    <t>ValProgFee</t>
+  </si>
+  <si>
+    <t>ValTxnFee</t>
+  </si>
+  <si>
+    <t>Fees: "Retainer info required, enter 0 if none"</t>
+  </si>
+  <si>
+    <t>The value can't be null for 'Retainer Fee Creditable'</t>
+  </si>
+  <si>
+    <t>The value can't be null for 'Progress Fee Creditable ?'</t>
+  </si>
+  <si>
+    <t>Select a transaction type value.</t>
+  </si>
+  <si>
+    <t>valWillThere</t>
+  </si>
+  <si>
+    <t>Pre-Pitch: Will there be a pitch?</t>
+  </si>
+  <si>
+    <t>ValHLComp</t>
+  </si>
+  <si>
+    <t>Pre-Pitch: Please identify Houlihan Lokey competition.</t>
+  </si>
+  <si>
+    <t>ValLockups</t>
+  </si>
+  <si>
+    <t>ValExisting</t>
+  </si>
+  <si>
+    <t>ValExistingRepeat</t>
+  </si>
+  <si>
+    <t>Pre-Pitch: Have you checked Salesforce for existing relationships?</t>
+  </si>
+  <si>
+    <t>Pre-Pitch: Existing or Repeat Client?</t>
+  </si>
+  <si>
+    <t>ValTAS</t>
+  </si>
+  <si>
+    <t>ValOutside</t>
+  </si>
+  <si>
+    <t>Pre-Pitch: If known, identify the name(s) of the client’s outside counsel and/or other advisors (If any)</t>
+  </si>
+  <si>
+    <t>Fairness Checklist: Is there a potential Fairness Opinion component to this assignment?</t>
+  </si>
+  <si>
+    <t>ValFairness</t>
+  </si>
+  <si>
+    <t>ValA</t>
+  </si>
+  <si>
+    <t>ValB</t>
+  </si>
+  <si>
+    <t>ValC</t>
+  </si>
+  <si>
+    <t>ValD</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Please confirm that a group head has approved prior to submitting to the committee.</t>
+  </si>
+  <si>
+    <t>valGroup</t>
+  </si>
+  <si>
+    <t>Pre-Pitch: Would the Opportunity benefit from TAS Assistance?</t>
+  </si>
+  <si>
+    <t>Pitched</t>
+  </si>
+  <si>
+    <t>Brian Miller</t>
+  </si>
+  <si>
+    <t>valUpdRetainer</t>
+  </si>
+  <si>
+    <t>120000.0</t>
+  </si>
+  <si>
+    <t>valUpdRetainerCred</t>
+  </si>
+  <si>
+    <t>FromAmt</t>
+  </si>
+  <si>
+    <t>ToAmt</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Transaction Overview</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Total Debt(MM)</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Valuation Expectations</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Current Status</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Company Description</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Real Estate Angle</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Ownership Structure &amp; Capital Structure</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Asia Angle</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Risk Factors</t>
+  </si>
+  <si>
+    <t>Opportunity Overview: Cross-border Angle</t>
+  </si>
+  <si>
+    <t>Financials: Have the financials been subject to an audit?</t>
+  </si>
+  <si>
+    <t>Pre-Pitch: Lockups on Future M&amp;A or Financing Work</t>
+  </si>
+  <si>
+    <t>Public Sensitivity: Please answer the Public M&amp;A question.</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>UpdEstValue</t>
+  </si>
+  <si>
+    <t>80.00</t>
+  </si>
+  <si>
+    <t>15.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -433,6 +636,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,11 +919,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,13 +1041,13 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -874,7 +1080,7 @@
         <v>18</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>38</v>
@@ -926,11 +1132,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,25 +1150,25 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -971,7 +1177,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1016,7 +1222,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
@@ -1047,7 +1253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1063,24 +1269,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
         <v>100</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>101</v>
-      </c>
-      <c r="C2" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1089,16 +1295,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:BP33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="BN2" sqref="BN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="95.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
@@ -1118,11 +1324,37 @@
     <col min="23" max="23" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="24" max="30" width="8.85546875" style="10"/>
     <col min="31" max="31" width="10.5703125" style="10" customWidth="1"/>
-    <col min="32" max="32" width="102.28515625" style="10" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="10"/>
+    <col min="32" max="32" width="32.42578125" style="10" customWidth="1"/>
+    <col min="33" max="33" width="17.42578125" style="10" customWidth="1"/>
+    <col min="34" max="34" width="15.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.5703125" style="9" customWidth="1"/>
+    <col min="37" max="38" width="13.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.7109375" style="10" customWidth="1"/>
+    <col min="47" max="47" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.85546875" style="10"/>
+    <col min="57" max="57" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="59" max="63" width="8.85546875" style="10"/>
+    <col min="64" max="68" width="14.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="69" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>57</v>
       </c>
@@ -1219,10 +1451,118 @@
       <c r="AF1" s="11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" ht="216.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="AN1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="AO1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS1" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="AU1" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="AV1" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AW1" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AX1" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY1" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="AZ1" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="BA1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="BB1" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="BC1" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="BE1" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="BF1" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="BG1" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="BH1" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="BI1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="BJ1" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="BK1" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="BL1" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="BM1" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN1" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="BO1" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="BP1" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:68" ht="216.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>9</v>
@@ -1231,7 +1571,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>60</v>
@@ -1254,7 +1594,7 @@
       <c r="K2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="5" t="s">
         <v>60</v>
       </c>
       <c r="M2" s="10" t="s">
@@ -1317,47 +1657,155 @@
       <c r="AF2" s="9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="AO2" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="AQ2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="AS2" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="AT2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="AU2" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="AW2" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AX2" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AY2" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="AZ2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="BA2" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="BB2" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="BC2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="BD2" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="BE2" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="BG2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="BH2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="BI2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="BJ2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="BK2" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="BL2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM2" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="BN2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="BO2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="BP2" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
     </row>
-    <row r="16" spans="1:32" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
     </row>
     <row r="17" spans="1:1" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>